<commit_message>
Aquisition session-range option, Individual Susceptibility updates
the period over which infusions were averaged to determine Acquire vs. NonAcquire was previously hard-coded. Now it's a setting at the top of the file. You indicate the session type (should be 'Training' unless someone's interested in the pre-training week), then can indicate whether to average across all sessions or whether to use the n first or last sessions.

PCA is now calculated within the same subgroups used for correlation analyses.

Z-scores  and subsequent analyses (correlation, PCA) are now only calculated within Acquirers

PCA 3D plot now matches Kevin's publication figure color scheme
</commit_message>
<xml_diff>
--- a/All Figures/Run_all_all_exclusions/Behavior Tables/run_all_exp_BE_inputData.xlsx
+++ b/All Figures/Run_all_all_exclusions/Behavior Tables/run_all_exp_BE_inputData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="57608" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="64809" uniqueCount="87">
   <si>
     <t>TagNumber</t>
   </si>
@@ -64246,7 +64246,7 @@
         <v>6</v>
       </c>
       <c r="Z801" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="802">
@@ -64326,7 +64326,7 @@
         <v>6</v>
       </c>
       <c r="Z802" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="803">
@@ -64406,7 +64406,7 @@
         <v>6</v>
       </c>
       <c r="Z803" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="804">
@@ -64486,7 +64486,7 @@
         <v>6</v>
       </c>
       <c r="Z804" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="805">
@@ -64566,7 +64566,7 @@
         <v>6</v>
       </c>
       <c r="Z805" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="806">
@@ -64646,7 +64646,7 @@
         <v>6</v>
       </c>
       <c r="Z806" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="807">
@@ -64726,7 +64726,7 @@
         <v>6</v>
       </c>
       <c r="Z807" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="808">
@@ -64806,7 +64806,7 @@
         <v>6</v>
       </c>
       <c r="Z808" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="809">
@@ -64886,7 +64886,7 @@
         <v>6</v>
       </c>
       <c r="Z809" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="810">
@@ -64966,7 +64966,7 @@
         <v>6</v>
       </c>
       <c r="Z810" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="811">
@@ -65046,7 +65046,7 @@
         <v>6</v>
       </c>
       <c r="Z811" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="812">
@@ -65126,7 +65126,7 @@
         <v>6</v>
       </c>
       <c r="Z812" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="813">
@@ -65206,7 +65206,7 @@
         <v>6</v>
       </c>
       <c r="Z813" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="814">
@@ -65286,7 +65286,7 @@
         <v>6</v>
       </c>
       <c r="Z814" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="815">
@@ -65366,7 +65366,7 @@
         <v>6</v>
       </c>
       <c r="Z815" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="816">
@@ -65446,7 +65446,7 @@
         <v>6</v>
       </c>
       <c r="Z816" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="817">
@@ -65526,7 +65526,7 @@
         <v>6</v>
       </c>
       <c r="Z817" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="818">
@@ -65606,7 +65606,7 @@
         <v>6</v>
       </c>
       <c r="Z818" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="819">
@@ -65686,7 +65686,7 @@
         <v>6</v>
       </c>
       <c r="Z819" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="820">
@@ -65766,7 +65766,7 @@
         <v>6</v>
       </c>
       <c r="Z820" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="821">
@@ -65846,7 +65846,7 @@
         <v>6</v>
       </c>
       <c r="Z821" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="822">
@@ -65926,7 +65926,7 @@
         <v>6</v>
       </c>
       <c r="Z822" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="823">

</xml_diff>